<commit_message>
Improve the EOQ Calculation, add the excel upload, handle some errors. Change the Homepage and the Team Page as well. Do some small error handlings. Back- and Frontend.
</commit_message>
<xml_diff>
--- a/reactdeterministicmodelslotsizing/reactdeterministicmodelslotsizing/src/assets/xlsx/1Import_Deterministic_Models.xlsx
+++ b/reactdeterministicmodelslotsizing/reactdeterministicmodelslotsizing/src/assets/xlsx/1Import_Deterministic_Models.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximilianstablum/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tamin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD3F1D6A-EA88-1E4D-AECC-14236BBCFE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA51291-87B2-43C6-B45E-EF0472D2C442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="500" windowWidth="28240" windowHeight="16340" xr2:uid="{934526B2-2149-0447-A048-FA636BDCBF06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{934526B2-2149-0447-A048-FA636BDCBF06}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Dropdown" sheetId="2" r:id="rId2"/>
+    <sheet name="Dropdown" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Template Deterministic Models Lot Sizing</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Order Costs:</t>
-  </si>
-  <si>
-    <t>Weeks per Year:</t>
   </si>
   <si>
     <t>Demand</t>
@@ -64,6 +61,15 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>This is a template for uploading planning data and the subsequent calculation of demand data. The fields Holding Costs and Order Costs must be filled with positive numbers for a meaningful calculation (negative not possible). The Demand can be filled from left to right according to the desired periods. It is important to stick to the same time interval during the entries of the data. Values between two and 100 periods are provided. By subsequently saving and uploading the template, both the EOQ and the Wagner Whitin can be calculated.</t>
+  </si>
+  <si>
+    <t>Time Interval</t>
   </si>
 </sst>
 </file>
@@ -214,15 +220,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -232,7 +243,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -251,9 +264,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -291,7 +304,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -397,7 +410,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -539,7 +552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -547,145 +560,796 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D94A4C1-A6CB-9E46-A745-866DB6BEF1B3}">
-  <dimension ref="B1:M8"/>
+  <dimension ref="B1:CY18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+    <row r="1" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="10"/>
-    </row>
-    <row r="3" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="9"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="9"/>
+      <c r="AU2" s="9"/>
+      <c r="AV2" s="9"/>
+      <c r="AW2" s="9"/>
+      <c r="AX2" s="9"/>
+      <c r="AY2" s="9"/>
+      <c r="AZ2" s="9"/>
+      <c r="BA2" s="9"/>
+      <c r="BB2" s="9"/>
+      <c r="BC2" s="9"/>
+      <c r="BD2" s="9"/>
+      <c r="BE2" s="9"/>
+      <c r="BF2" s="9"/>
+      <c r="BG2" s="9"/>
+      <c r="BH2" s="9"/>
+      <c r="BI2" s="9"/>
+      <c r="BJ2" s="9"/>
+      <c r="BK2" s="9"/>
+      <c r="BL2" s="9"/>
+      <c r="BM2" s="9"/>
+      <c r="BN2" s="9"/>
+      <c r="BO2" s="9"/>
+      <c r="BP2" s="9"/>
+      <c r="BQ2" s="9"/>
+      <c r="BR2" s="9"/>
+      <c r="BS2" s="9"/>
+      <c r="BT2" s="9"/>
+      <c r="BU2" s="9"/>
+      <c r="BV2" s="9"/>
+      <c r="BW2" s="9"/>
+      <c r="BX2" s="9"/>
+      <c r="BY2" s="9"/>
+      <c r="BZ2" s="9"/>
+      <c r="CA2" s="9"/>
+      <c r="CB2" s="9"/>
+      <c r="CC2" s="9"/>
+      <c r="CD2" s="9"/>
+      <c r="CE2" s="9"/>
+      <c r="CF2" s="9"/>
+      <c r="CG2" s="9"/>
+      <c r="CH2" s="9"/>
+      <c r="CI2" s="9"/>
+      <c r="CJ2" s="9"/>
+      <c r="CK2" s="9"/>
+      <c r="CL2" s="9"/>
+      <c r="CM2" s="9"/>
+      <c r="CN2" s="9"/>
+      <c r="CO2" s="9"/>
+      <c r="CP2" s="9"/>
+      <c r="CQ2" s="9"/>
+      <c r="CR2" s="9"/>
+      <c r="CS2" s="9"/>
+      <c r="CT2" s="9"/>
+      <c r="CU2" s="9"/>
+      <c r="CV2" s="9"/>
+      <c r="CW2" s="9"/>
+      <c r="CX2" s="9"/>
+      <c r="CY2" s="10"/>
+    </row>
+    <row r="3" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="7"/>
+      <c r="CY3" s="3"/>
+    </row>
+    <row r="4" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="C4" s="7"/>
+      <c r="CY4" s="3"/>
+    </row>
+    <row r="5" spans="2:103" x14ac:dyDescent="0.35">
+      <c r="B5" s="2"/>
+      <c r="CY5" s="3"/>
+    </row>
+    <row r="6" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>2</v>
+      </c>
+      <c r="E6" s="8">
         <v>3</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="8">
+        <v>4</v>
+      </c>
+      <c r="G6" s="8">
+        <v>5</v>
+      </c>
+      <c r="H6" s="8">
+        <v>6</v>
+      </c>
+      <c r="I6" s="8">
+        <v>7</v>
+      </c>
+      <c r="J6" s="8">
+        <v>8</v>
+      </c>
+      <c r="K6" s="8">
+        <v>9</v>
+      </c>
+      <c r="L6" s="8">
+        <v>10</v>
+      </c>
+      <c r="M6" s="8">
+        <v>11</v>
+      </c>
+      <c r="N6" s="8">
+        <v>12</v>
+      </c>
+      <c r="O6" s="8">
+        <v>13</v>
+      </c>
+      <c r="P6" s="8">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>15</v>
+      </c>
+      <c r="R6" s="8">
+        <v>16</v>
+      </c>
+      <c r="S6" s="8">
+        <v>17</v>
+      </c>
+      <c r="T6" s="8">
+        <v>18</v>
+      </c>
+      <c r="U6" s="8">
+        <v>19</v>
+      </c>
+      <c r="V6" s="8">
+        <v>20</v>
+      </c>
+      <c r="W6" s="8">
+        <v>21</v>
+      </c>
+      <c r="X6" s="8">
+        <v>22</v>
+      </c>
+      <c r="Y6" s="8">
+        <v>23</v>
+      </c>
+      <c r="Z6" s="8">
+        <v>24</v>
+      </c>
+      <c r="AA6" s="8">
+        <v>25</v>
+      </c>
+      <c r="AB6" s="8">
+        <v>26</v>
+      </c>
+      <c r="AC6" s="8">
+        <v>27</v>
+      </c>
+      <c r="AD6" s="8">
+        <v>28</v>
+      </c>
+      <c r="AE6" s="8">
+        <v>29</v>
+      </c>
+      <c r="AF6" s="8">
+        <v>30</v>
+      </c>
+      <c r="AG6" s="8">
+        <v>31</v>
+      </c>
+      <c r="AH6" s="8">
+        <v>32</v>
+      </c>
+      <c r="AI6" s="8">
+        <v>33</v>
+      </c>
+      <c r="AJ6" s="8">
+        <v>34</v>
+      </c>
+      <c r="AK6" s="8">
+        <v>35</v>
+      </c>
+      <c r="AL6" s="8">
+        <v>36</v>
+      </c>
+      <c r="AM6" s="8">
+        <v>37</v>
+      </c>
+      <c r="AN6" s="8">
+        <v>38</v>
+      </c>
+      <c r="AO6" s="8">
+        <v>39</v>
+      </c>
+      <c r="AP6" s="8">
+        <v>40</v>
+      </c>
+      <c r="AQ6" s="8">
+        <v>41</v>
+      </c>
+      <c r="AR6" s="8">
+        <v>42</v>
+      </c>
+      <c r="AS6" s="8">
+        <v>43</v>
+      </c>
+      <c r="AT6" s="8">
+        <v>44</v>
+      </c>
+      <c r="AU6" s="8">
+        <v>45</v>
+      </c>
+      <c r="AV6" s="8">
+        <v>46</v>
+      </c>
+      <c r="AW6" s="8">
+        <v>47</v>
+      </c>
+      <c r="AX6" s="8">
+        <v>48</v>
+      </c>
+      <c r="AY6" s="8">
+        <v>49</v>
+      </c>
+      <c r="AZ6" s="8">
+        <v>50</v>
+      </c>
+      <c r="BA6" s="8">
+        <v>51</v>
+      </c>
+      <c r="BB6" s="8">
+        <v>52</v>
+      </c>
+      <c r="BC6" s="8">
+        <v>53</v>
+      </c>
+      <c r="BD6" s="8">
+        <v>54</v>
+      </c>
+      <c r="BE6" s="8">
+        <v>55</v>
+      </c>
+      <c r="BF6" s="8">
+        <v>56</v>
+      </c>
+      <c r="BG6" s="8">
+        <v>57</v>
+      </c>
+      <c r="BH6" s="8">
+        <v>58</v>
+      </c>
+      <c r="BI6" s="8">
+        <v>59</v>
+      </c>
+      <c r="BJ6" s="8">
+        <v>60</v>
+      </c>
+      <c r="BK6" s="8">
+        <v>61</v>
+      </c>
+      <c r="BL6" s="8">
+        <v>62</v>
+      </c>
+      <c r="BM6" s="8">
+        <v>63</v>
+      </c>
+      <c r="BN6" s="8">
+        <v>64</v>
+      </c>
+      <c r="BO6" s="8">
+        <v>65</v>
+      </c>
+      <c r="BP6" s="8">
+        <v>66</v>
+      </c>
+      <c r="BQ6" s="8">
+        <v>67</v>
+      </c>
+      <c r="BR6" s="8">
+        <v>68</v>
+      </c>
+      <c r="BS6" s="8">
+        <v>69</v>
+      </c>
+      <c r="BT6" s="8">
+        <v>70</v>
+      </c>
+      <c r="BU6" s="8">
+        <v>71</v>
+      </c>
+      <c r="BV6" s="8">
+        <v>72</v>
+      </c>
+      <c r="BW6" s="8">
+        <v>73</v>
+      </c>
+      <c r="BX6" s="8">
+        <v>74</v>
+      </c>
+      <c r="BY6" s="8">
+        <v>75</v>
+      </c>
+      <c r="BZ6" s="8">
+        <v>76</v>
+      </c>
+      <c r="CA6" s="8">
+        <v>77</v>
+      </c>
+      <c r="CB6" s="8">
+        <v>78</v>
+      </c>
+      <c r="CC6" s="8">
+        <v>79</v>
+      </c>
+      <c r="CD6" s="8">
+        <v>80</v>
+      </c>
+      <c r="CE6" s="8">
+        <v>81</v>
+      </c>
+      <c r="CF6" s="8">
+        <v>82</v>
+      </c>
+      <c r="CG6" s="8">
+        <v>83</v>
+      </c>
+      <c r="CH6" s="8">
+        <v>84</v>
+      </c>
+      <c r="CI6" s="8">
+        <v>85</v>
+      </c>
+      <c r="CJ6" s="8">
+        <v>86</v>
+      </c>
+      <c r="CK6" s="8">
+        <v>87</v>
+      </c>
+      <c r="CL6" s="8">
+        <v>88</v>
+      </c>
+      <c r="CM6" s="8">
+        <v>89</v>
+      </c>
+      <c r="CN6" s="8">
+        <v>90</v>
+      </c>
+      <c r="CO6" s="8">
+        <v>91</v>
+      </c>
+      <c r="CP6" s="8">
+        <v>92</v>
+      </c>
+      <c r="CQ6" s="8">
+        <v>93</v>
+      </c>
+      <c r="CR6" s="8">
+        <v>94</v>
+      </c>
+      <c r="CS6" s="8">
+        <v>95</v>
+      </c>
+      <c r="CT6" s="8">
+        <v>96</v>
+      </c>
+      <c r="CU6" s="8">
+        <v>97</v>
+      </c>
+      <c r="CV6" s="8">
+        <v>98</v>
+      </c>
+      <c r="CW6" s="8">
+        <v>99</v>
+      </c>
+      <c r="CX6" s="8">
+        <v>100</v>
+      </c>
+      <c r="CY6" s="3"/>
+    </row>
+    <row r="7" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AK7" s="7"/>
+      <c r="AL7" s="7"/>
+      <c r="AM7" s="7"/>
+      <c r="AN7" s="7"/>
+      <c r="AO7" s="7"/>
+      <c r="AP7" s="7"/>
+      <c r="AQ7" s="7"/>
+      <c r="AR7" s="7"/>
+      <c r="AS7" s="7"/>
+      <c r="AT7" s="7"/>
+      <c r="AU7" s="7"/>
+      <c r="AV7" s="7"/>
+      <c r="AW7" s="7"/>
+      <c r="AX7" s="7"/>
+      <c r="AY7" s="7"/>
+      <c r="AZ7" s="7"/>
+      <c r="BA7" s="7"/>
+      <c r="BB7" s="7"/>
+      <c r="BC7" s="7"/>
+      <c r="BD7" s="7"/>
+      <c r="BE7" s="7"/>
+      <c r="BF7" s="7"/>
+      <c r="BG7" s="7"/>
+      <c r="BH7" s="7"/>
+      <c r="BI7" s="7"/>
+      <c r="BJ7" s="7"/>
+      <c r="BK7" s="7"/>
+      <c r="BL7" s="7"/>
+      <c r="BM7" s="7"/>
+      <c r="BN7" s="7"/>
+      <c r="BO7" s="7"/>
+      <c r="BP7" s="7"/>
+      <c r="BQ7" s="7"/>
+      <c r="BR7" s="7"/>
+      <c r="BS7" s="7"/>
+      <c r="BT7" s="7"/>
+      <c r="BU7" s="7"/>
+      <c r="BV7" s="7"/>
+      <c r="BW7" s="7"/>
+      <c r="BX7" s="7"/>
+      <c r="BY7" s="7"/>
+      <c r="BZ7" s="7"/>
+      <c r="CA7" s="7"/>
+      <c r="CB7" s="7"/>
+      <c r="CC7" s="7"/>
+      <c r="CD7" s="7"/>
+      <c r="CE7" s="7"/>
+      <c r="CF7" s="7"/>
+      <c r="CG7" s="7"/>
+      <c r="CH7" s="7"/>
+      <c r="CI7" s="7"/>
+      <c r="CJ7" s="7"/>
+      <c r="CK7" s="7"/>
+      <c r="CL7" s="7"/>
+      <c r="CM7" s="7"/>
+      <c r="CN7" s="7"/>
+      <c r="CO7" s="7"/>
+      <c r="CP7" s="7"/>
+      <c r="CQ7" s="7"/>
+      <c r="CR7" s="7"/>
+      <c r="CS7" s="7"/>
+      <c r="CT7" s="7"/>
+      <c r="CU7" s="7"/>
+      <c r="CV7" s="7"/>
+      <c r="CW7" s="7"/>
+      <c r="CX7" s="7"/>
+      <c r="CY7" s="3"/>
+    </row>
+    <row r="8" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="5"/>
+      <c r="AJ8" s="5"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="5"/>
+      <c r="AN8" s="5"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="5"/>
+      <c r="AQ8" s="5"/>
+      <c r="AR8" s="5"/>
+      <c r="AS8" s="5"/>
+      <c r="AT8" s="5"/>
+      <c r="AU8" s="5"/>
+      <c r="AV8" s="5"/>
+      <c r="AW8" s="5"/>
+      <c r="AX8" s="5"/>
+      <c r="AY8" s="5"/>
+      <c r="AZ8" s="5"/>
+      <c r="BA8" s="5"/>
+      <c r="BB8" s="5"/>
+      <c r="BC8" s="5"/>
+      <c r="BD8" s="5"/>
+      <c r="BE8" s="5"/>
+      <c r="BF8" s="5"/>
+      <c r="BG8" s="5"/>
+      <c r="BH8" s="5"/>
+      <c r="BI8" s="5"/>
+      <c r="BJ8" s="5"/>
+      <c r="BK8" s="5"/>
+      <c r="BL8" s="5"/>
+      <c r="BM8" s="5"/>
+      <c r="BN8" s="5"/>
+      <c r="BO8" s="5"/>
+      <c r="BP8" s="5"/>
+      <c r="BQ8" s="5"/>
+      <c r="BR8" s="5"/>
+      <c r="BS8" s="5"/>
+      <c r="BT8" s="5"/>
+      <c r="BU8" s="5"/>
+      <c r="BV8" s="5"/>
+      <c r="BW8" s="5"/>
+      <c r="BX8" s="5"/>
+      <c r="BY8" s="5"/>
+      <c r="BZ8" s="5"/>
+      <c r="CA8" s="5"/>
+      <c r="CB8" s="5"/>
+      <c r="CC8" s="5"/>
+      <c r="CD8" s="5"/>
+      <c r="CE8" s="5"/>
+      <c r="CF8" s="5"/>
+      <c r="CG8" s="5"/>
+      <c r="CH8" s="5"/>
+      <c r="CI8" s="5"/>
+      <c r="CJ8" s="5"/>
+      <c r="CK8" s="5"/>
+      <c r="CL8" s="5"/>
+      <c r="CM8" s="5"/>
+      <c r="CN8" s="5"/>
+      <c r="CO8" s="5"/>
+      <c r="CP8" s="5"/>
+      <c r="CQ8" s="5"/>
+      <c r="CR8" s="5"/>
+      <c r="CS8" s="5"/>
+      <c r="CT8" s="5"/>
+      <c r="CU8" s="5"/>
+      <c r="CV8" s="5"/>
+      <c r="CW8" s="5"/>
+      <c r="CX8" s="5"/>
+      <c r="CY8" s="6"/>
+    </row>
+    <row r="10" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="2:103" x14ac:dyDescent="0.35">
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="13"/>
+    </row>
+    <row r="12" spans="2:103" x14ac:dyDescent="0.35">
+      <c r="B12" s="2"/>
+      <c r="C12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="3"/>
+    </row>
+    <row r="13" spans="2:103" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="2:103" x14ac:dyDescent="0.35">
+      <c r="B14" s="2"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="2:103" x14ac:dyDescent="0.35">
+      <c r="B15" s="2"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="2:103" x14ac:dyDescent="0.35">
+      <c r="B16" s="2"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B17" s="2"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="C12:L17"/>
   </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Value &gt;= 0" prompt=" " sqref="C7:CX7" xr:uid="{1607BC2B-8A02-42E3-BD6D-13925C8DACA2}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Holding Costs" prompt="Enter positive values._x000a_" sqref="C3" xr:uid="{1404C1DD-CE6A-4DCD-9F5C-8E4F7F055284}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Order Costs" prompt="Enter positive values._x000a_" sqref="C4" xr:uid="{4AFAB84C-761E-4BE2-9E03-5628B40DF5A3}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation showDropDown="1" showErrorMessage="1" promptTitle="Timeinterval" prompt="Select a value from the dropdown." sqref="C5" xr:uid="{C13BA546-D03D-314E-A765-D53CF0DAC9D2}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C13BA546-D03D-314E-A765-D53CF0DAC9D2}">
-          <x14:formula1>
-            <xm:f>Dropdown!$A$2:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>C5</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -697,31 +1361,31 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some minor bug fixes
</commit_message>
<xml_diff>
--- a/reactdeterministicmodelslotsizing/reactdeterministicmodelslotsizing/src/assets/xlsx/1Import_Deterministic_Models.xlsx
+++ b/reactdeterministicmodelslotsizing/reactdeterministicmodelslotsizing/src/assets/xlsx/1Import_Deterministic_Models.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tamin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tamin\workspace\deterministicModelsLotSizing\DeterministicModelsLotSizing\reactdeterministicmodelslotsizing\reactdeterministicmodelslotsizing\src\assets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA51291-87B2-43C6-B45E-EF0472D2C442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F4C64B-ABF7-46A1-82B9-0EED8F2F9261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{934526B2-2149-0447-A048-FA636BDCBF06}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>Holding Costs:</t>
   </si>
   <si>
-    <t>Order Costs:</t>
-  </si>
-  <si>
     <t>Demand</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Time Interval</t>
+  </si>
+  <si>
+    <t>Setup Costs:</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="B1:CY18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -689,7 +689,7 @@
     </row>
     <row r="4" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7"/>
       <c r="CY4" s="3"/>
@@ -700,7 +700,7 @@
     </row>
     <row r="6" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="8">
         <v>1</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="7" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1217,7 +1217,7 @@
     <row r="10" spans="2:103" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="2:103" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -1234,7 +1234,7 @@
     <row r="12" spans="2:103" x14ac:dyDescent="0.35">
       <c r="B12" s="2"/>
       <c r="C12" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -1365,27 +1365,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>